<commit_message>
Atualizando o arquivo jogos.xlsx com novas informações em 2025-01-08 18:46:00
</commit_message>
<xml_diff>
--- a/Data/jogos.xlsx
+++ b/Data/jogos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2215,6 +2215,28 @@
         </is>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Incompleto</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>PS3</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Zerar</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizando o arquivo jogos.xlsx com novas informações em 2025-01-08 19:01:29
</commit_message>
<xml_diff>
--- a/Data/jogos.xlsx
+++ b/Data/jogos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2196,42 +2196,20 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>teste de jogo ps5</t>
+          <t>GTA Vice City</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Completo</t>
+          <t>em progresso</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>PS5</t>
+          <t>PC</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
-        <is>
-          <t>Concluído</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Incompleto</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>PS3</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
         <is>
           <t>Zerar</t>
         </is>

</xml_diff>